<commit_message>
Bug en el exportador de ReporteOdometros.xlsx
</commit_message>
<xml_diff>
--- a/Logictracker/Logictracker/src/Web/Logictracker/Logictracker.Web/ExcelTemplate/Logictracker/ReporteOdometros.xlsx
+++ b/Logictracker/Logictracker/src/Web/Logictracker/Logictracker.Web/ExcelTemplate/Logictracker/ReporteOdometros.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorio\LogicTracker\Logictracker\Logictracker\src\Web\Logictracker\Logictracker.Web\ExcelTemplate\Logictracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias Alfano\Source\Repos\Logictracker 4.0\Logictracker\Logictracker\src\Web\Logictracker\Logictracker.Web\ExcelTemplate\Logictracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,6 +31,7 @@
     <definedName name="PATENTE">Informe!$D$9</definedName>
     <definedName name="REFERENCIA">Informe!$G$9</definedName>
     <definedName name="RESPONSABLE">Informe!$F$9</definedName>
+    <definedName name="T_FALT">Informe!$L$9</definedName>
     <definedName name="T_REF">Informe!$I$9</definedName>
     <definedName name="Titulo">Informe!$C$1</definedName>
     <definedName name="ULTIMO_UPDATE">Informe!$O$9</definedName>
@@ -1047,8 +1048,8 @@
   </sheetPr>
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>